<commit_message>
add hasDaschUrl to sgv:Dataset
</commit_message>
<xml_diff>
--- a/ontology/SGV/dsp/Resources.xlsx
+++ b/ontology/SGV/dsp/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julienraemy/Documents/GitHub/pia-data-model/ontology/SGV/dsp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195812D8-2FCC-0742-882C-4BD3E903954C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90716430-A402-CA49-A5CD-3293DEAFB853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="8" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" activeTab="3" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="134">
   <si>
     <t>Cardinality</t>
   </si>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:B41"/>
+      <selection activeCell="A30" sqref="A30:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1470,15 +1470,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD91F824-1F3E-7E48-A5CC-061BC01D3E73}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1660,6 +1661,14 @@
       </c>
       <c r="B22" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2447,7 +2456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CE4E426-8F65-E04A-9C4A-1F73D935C2CC}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I10:I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>